<commit_message>
Define a 1-1 relationship: User and Employee
</commit_message>
<xml_diff>
--- a/storage/app/import/users.xlsx
+++ b/storage/app/import/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkukuh/Sites/memfis/storage/app/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC6B741-8681-3642-9967-1D8068800134}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B71983-7899-F240-976C-6289B697DA40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G115" sqref="G115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1872,6 +1872,9 @@
       </c>
     </row>
     <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>17043000</v>
+      </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Add 1 PPC employee
</commit_message>
<xml_diff>
--- a/storage/app/import/users.xlsx
+++ b/storage/app/import/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkukuh/Sites/memfis/storage/app/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A24FF-0F83-5A40-829B-3BD4AC90DFD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA7C0DE-01E0-1C4F-B660-848FD4A986CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="402">
   <si>
     <t>NRP</t>
   </si>
@@ -1220,6 +1220,12 @@
   </si>
   <si>
     <t>00000000</t>
+  </si>
+  <si>
+    <t>muhwahyudi@ptmmf.co.id</t>
+  </si>
+  <si>
+    <t>MUHAMMAD WAHYUDI</t>
   </si>
 </sst>
 </file>
@@ -1721,11 +1727,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2131,10 +2138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D181"/>
+  <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4353,6 +4360,17 @@
       </c>
       <c r="D181" t="s">
         <v>398</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B182" t="s">
+        <v>401</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>